<commit_message>
Update interview armour budgett.xlsx
forgot to add the links!
</commit_message>
<xml_diff>
--- a/interview armour budgett.xlsx
+++ b/interview armour budgett.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eilidh\Documents\GitHub\Interview_Armour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDDB773-D778-49CC-A8A4-1132E3B39FA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABF63C4-D324-4524-8D1E-8B58F5B3E12B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19932" yWindow="4932" windowWidth="6168" windowHeight="5208" xr2:uid="{5E714FC1-DCA5-48B7-8CF1-557A87F09F23}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">Budget - Interview armour </t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>slide buckles</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/dp/9553548296/?coliid=I1WUO41FZR9AN4&amp;colid=4EYVC5LB6BFN&amp;psc=0&amp;ref_=lv_ov_lig_dp_it</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/dp/B00MNKUIT8/?coliid=IG139WPE5GBEE&amp;colid=4EYVC5LB6BFN&amp;psc=1&amp;ref_=lv_ov_lig_dp_it</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/dp/B00J3YAK2M/?coliid=IZ7CDRDN889D&amp;colid=4EYVC5LB6BFN&amp;psc=0&amp;ref_=lv_ov_lig_dp_it</t>
   </si>
 </sst>
 </file>
@@ -432,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360AA32C-0A72-4738-9C28-EF2D81EDD76E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,6 +564,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -570,6 +582,9 @@
         <f t="shared" ref="D9:D10" si="1">B9*C9</f>
         <v>1.48</v>
       </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -584,6 +599,9 @@
       <c r="D10">
         <f t="shared" si="1"/>
         <v>1.54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>